<commit_message>
podmiana rysunkow 2.1 i 2.2, powiekszenie rysunku 3.1
</commit_message>
<xml_diff>
--- a/wykresy.xlsx
+++ b/wykresy.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="13740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Testy jednostkowe 1" sheetId="1" r:id="rId1"/>
     <sheet name="struktura aplikacji podstawowej" sheetId="2" r:id="rId2"/>
     <sheet name="schemat aplikacji poprawionej" sheetId="3" r:id="rId3"/>
-    <sheet name="Arkusz1" sheetId="4" r:id="rId4"/>
+    <sheet name="udzial dystrybucji" sheetId="4" r:id="rId4"/>
+    <sheet name="udzial w rynku" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t xml:space="preserve">Wersja pierwotna </t>
   </si>
@@ -103,6 +104,42 @@
   </si>
   <si>
     <t>ążęćń</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>Windows Phone</t>
+  </si>
+  <si>
+    <t>Symbian</t>
+  </si>
+  <si>
+    <t>Java ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackBerry </t>
+  </si>
+  <si>
+    <t>Kindle</t>
+  </si>
+  <si>
+    <t>Inne</t>
+  </si>
+  <si>
+    <t>Swiat</t>
+  </si>
+  <si>
+    <t>Nie wiem</t>
+  </si>
+  <si>
+    <t>Inny</t>
+  </si>
+  <si>
+    <t>Polska</t>
   </si>
 </sst>
 </file>
@@ -213,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -232,7 +269,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -294,11 +331,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="134089344"/>
-        <c:axId val="135160192"/>
+        <c:axId val="120945280"/>
+        <c:axId val="120951168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134089344"/>
+        <c:axId val="120945280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -307,7 +344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135160192"/>
+        <c:crossAx val="120951168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -315,7 +352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135160192"/>
+        <c:axId val="120951168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,7 +363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134089344"/>
+        <c:crossAx val="120945280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -346,7 +383,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -417,11 +454,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="135179648"/>
-        <c:axId val="136320128"/>
+        <c:axId val="120970624"/>
+        <c:axId val="121242752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135179648"/>
+        <c:axId val="120970624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136320128"/>
+        <c:crossAx val="121242752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -438,7 +475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136320128"/>
+        <c:axId val="121242752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135179648"/>
+        <c:crossAx val="120970624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -469,7 +506,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -533,11 +570,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="136343936"/>
-        <c:axId val="136345472"/>
+        <c:axId val="121266560"/>
+        <c:axId val="121268096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136343936"/>
+        <c:axId val="121266560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136345472"/>
+        <c:crossAx val="121268096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -554,7 +591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136345472"/>
+        <c:axId val="121268096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136343936"/>
+        <c:crossAx val="121266560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -585,7 +622,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -658,11 +695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="63751680"/>
-        <c:axId val="63753216"/>
+        <c:axId val="121287808"/>
+        <c:axId val="121289344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63751680"/>
+        <c:axId val="121287808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63753216"/>
+        <c:crossAx val="121289344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -679,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63753216"/>
+        <c:axId val="121289344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63751680"/>
+        <c:crossAx val="121287808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -710,7 +747,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -750,7 +787,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$J$4:$J$9</c:f>
+              <c:f>'udzial dystrybucji'!$J$4:$J$9</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -776,7 +813,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$K$4:$K$9</c:f>
+              <c:f>'udzial dystrybucji'!$K$4:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -825,6 +862,290 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'udzial w rynku'!$A$1:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>iOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Windows Phone</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Symbian</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Java ME</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BlackBerry </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Kindle</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Inne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'udzial w rynku'!$B$1:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.53539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.15E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="134432640"/>
+        <c:axId val="134431488"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="134431488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134432640"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="134432640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134431488"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'udzial w rynku'!$J$1:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Windows Phone</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iOS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nie wiem</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BlackBerry </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Inny</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'udzial w rynku'!$K$1:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="131167360"/>
+        <c:axId val="131168896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="131167360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131168896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="131168896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131167360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -7767,6 +8088,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B19:E28" totalsRowShown="0">
   <autoFilter ref="B19:E28"/>
@@ -7781,9 +8167,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7821,7 +8207,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -7893,7 +8279,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8069,7 +8455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
@@ -8521,4 +8907,134 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.35580000000000001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.4400000000000002E-2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.15E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>